<commit_message>
g - o moves, gen 4
</commit_message>
<xml_diff>
--- a/documents/pokedex/pokedex.xlsx
+++ b/documents/pokedex/pokedex.xlsx
@@ -79,7 +79,7 @@
     <t xml:space="preserve">Mime Jr.</t>
   </si>
   <si>
-    <t xml:space="preserve">Mr Mime</t>
+    <t xml:space="preserve">Mr. Mime</t>
   </si>
   <si>
     <t xml:space="preserve">Jarrater</t>
@@ -1451,7 +1451,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1633,11 +1633,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:axId val="43436521"/>
-        <c:axId val="80760358"/>
+        <c:axId val="38892732"/>
+        <c:axId val="32972325"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="43436521"/>
+        <c:axId val="38892732"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1665,14 +1665,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80760358"/>
+        <c:crossAx val="32972325"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80760358"/>
+        <c:axId val="32972325"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1709,7 +1709,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43436521"/>
+        <c:crossAx val="38892732"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1767,9 +1767,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>149400</xdr:colOff>
+      <xdr:colOff>149040</xdr:colOff>
       <xdr:row>83</xdr:row>
-      <xdr:rowOff>48240</xdr:rowOff>
+      <xdr:rowOff>47880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1778,7 +1778,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="78840" y="11362320"/>
-        <a:ext cx="5763240" cy="3232440"/>
+        <a:ext cx="5762880" cy="3232080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1798,8 +1798,8 @@
   </sheetPr>
   <dimension ref="A1:AY1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G96" activeCellId="0" sqref="G96"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K49" activeCellId="0" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1833,7 +1833,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="9.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="10.46"/>

</xml_diff>

<commit_message>
pokedex evolution and obtainable
</commit_message>
<xml_diff>
--- a/documents/pokedex/pokedex.xlsx
+++ b/documents/pokedex/pokedex.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="237">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -199,15 +199,15 @@
     <t xml:space="preserve">Route 6, 9</t>
   </si>
   <si>
+    <t xml:space="preserve">Forest</t>
+  </si>
+  <si>
     <t xml:space="preserve">Garden, Route 5</t>
   </si>
   <si>
     <t xml:space="preserve">Garden</t>
   </si>
   <si>
-    <t xml:space="preserve">Forest</t>
-  </si>
-  <si>
     <t xml:space="preserve">Route 3, 4</t>
   </si>
   <si>
@@ -403,12 +403,12 @@
     <t xml:space="preserve">Sandy Cave</t>
   </si>
   <si>
+    <t xml:space="preserve">Upward Pass</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ranch</t>
   </si>
   <si>
-    <t xml:space="preserve">Upward Pass</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lucent Cavern</t>
   </si>
   <si>
@@ -568,6 +568,9 @@
     <t xml:space="preserve">Desert</t>
   </si>
   <si>
+    <t xml:space="preserve">Sandy Cave, Lucent Cavern</t>
+  </si>
+  <si>
     <t xml:space="preserve">Icy pass, Route 17</t>
   </si>
   <si>
@@ -700,6 +703,9 @@
     <t xml:space="preserve">Route 19</t>
   </si>
   <si>
+    <t xml:space="preserve">Only one</t>
+  </si>
+  <si>
     <t xml:space="preserve">Types</t>
   </si>
   <si>
@@ -716,6 +722,9 @@
   </si>
   <si>
     <t xml:space="preserve">To insert from later gens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unobtainable</t>
   </si>
   <si>
     <t xml:space="preserve">Chandelure</t>
@@ -1333,27 +1342,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="28" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="28" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="28" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1414,326 +1423,64 @@
   </cellStyles>
   <dxfs count="20">
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFFFFFFF"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF08030"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFFFFFFF"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF6890F0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="false" diagonalDown="false">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <diagonal/>
-      </border>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFFFFFFF"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF78C850"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFFFFFFF"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA040A0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="false" diagonalDown="false">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <diagonal/>
-      </border>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFFFFFFF"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8D030"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFFFFFFF"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE0C068"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFFFFFFF"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF85888"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFFFFFFF"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB8A038"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="false" diagonalDown="false">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <diagonal/>
-      </border>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFFFFFFF"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF98D8D8"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFFFFFFF"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA8B820"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFFFFFFF"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7038F8"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFFFFFFF"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF705898"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFFFFFFF"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF705848"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFFFFFFF"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB8B8D0"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFFFFFFF"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEE99AC"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFFFFFFF"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA890F0"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFFFFFFF"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC03028"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <color rgb="FFFFFFFF"/>
-        <sz val="11"/>
-        <u val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA8A878"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBBE33D"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="false" diagonalDown="false">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <diagonal/>
-      </border>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
     </dxf>
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-        <sz val="11"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3838"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="false" diagonalDown="false">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <diagonal/>
-      </border>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
     </dxf>
   </dxfs>
   <colors>
@@ -1981,11 +1728,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:axId val="68782378"/>
-        <c:axId val="61972041"/>
+        <c:axId val="73046543"/>
+        <c:axId val="59031602"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68782378"/>
+        <c:axId val="73046543"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2013,14 +1760,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61972041"/>
+        <c:crossAx val="59031602"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61972041"/>
+        <c:axId val="59031602"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2057,7 +1804,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68782378"/>
+        <c:crossAx val="73046543"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2115,9 +1862,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>148320</xdr:colOff>
+      <xdr:colOff>147960</xdr:colOff>
       <xdr:row>83</xdr:row>
-      <xdr:rowOff>47160</xdr:rowOff>
+      <xdr:rowOff>46800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2126,7 +1873,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="78840" y="11362320"/>
-        <a:ext cx="5762160" cy="3231360"/>
+        <a:ext cx="5761800" cy="3231000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2146,8 +1893,8 @@
   </sheetPr>
   <dimension ref="A1:AY1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AU27" activeCellId="0" sqref="AU27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2160,7 +1907,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.24"/>
@@ -2182,14 +1929,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="12.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="23.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="12.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="9.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="18.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="12.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="10.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="17.55"/>
@@ -2794,25 +2541,27 @@
       </c>
       <c r="W5" s="11"/>
       <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
+      <c r="Y5" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="Z5" s="11"/>
       <c r="AA5" s="11" t="s">
         <v>57</v>
       </c>
       <c r="AB5" s="11"/>
       <c r="AC5" s="11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AD5" s="11"/>
       <c r="AE5" s="11"/>
       <c r="AF5" s="11"/>
       <c r="AG5" s="11"/>
       <c r="AH5" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AI5" s="12"/>
       <c r="AJ5" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AK5" s="12"/>
       <c r="AL5" s="11" t="s">
@@ -2820,7 +2569,7 @@
       </c>
       <c r="AM5" s="12"/>
       <c r="AN5" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AO5" s="12"/>
       <c r="AP5" s="11" t="s">
@@ -3098,44 +2847,80 @@
         <v>72</v>
       </c>
       <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
+      <c r="N10" s="20" t="s">
+        <v>72</v>
+      </c>
       <c r="O10" s="21"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
+      <c r="P10" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q10" s="20" t="s">
+        <v>72</v>
+      </c>
       <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="20"/>
+      <c r="S10" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="T10" s="20" t="s">
+        <v>72</v>
+      </c>
       <c r="U10" s="20"/>
       <c r="V10" s="20"/>
-      <c r="W10" s="20"/>
-      <c r="X10" s="20"/>
+      <c r="W10" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="X10" s="20" t="s">
+        <v>72</v>
+      </c>
       <c r="Y10" s="20"/>
-      <c r="Z10" s="20"/>
+      <c r="Z10" s="20" t="s">
+        <v>72</v>
+      </c>
       <c r="AA10" s="20"/>
-      <c r="AB10" s="20"/>
+      <c r="AB10" s="20" t="s">
+        <v>72</v>
+      </c>
       <c r="AC10" s="20"/>
-      <c r="AD10" s="20"/>
+      <c r="AD10" s="20" t="s">
+        <v>72</v>
+      </c>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20"/>
       <c r="AG10" s="20"/>
       <c r="AH10" s="20"/>
-      <c r="AI10" s="21"/>
+      <c r="AI10" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AJ10" s="20"/>
-      <c r="AK10" s="21"/>
+      <c r="AK10" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AL10" s="20"/>
-      <c r="AM10" s="21"/>
+      <c r="AM10" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AN10" s="20"/>
-      <c r="AO10" s="21"/>
+      <c r="AO10" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AP10" s="20"/>
-      <c r="AQ10" s="21"/>
+      <c r="AQ10" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AR10" s="20"/>
-      <c r="AS10" s="21"/>
+      <c r="AS10" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AT10" s="20"/>
       <c r="AU10" s="21"/>
       <c r="AV10" s="20"/>
-      <c r="AW10" s="21"/>
+      <c r="AW10" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AX10" s="20"/>
-      <c r="AY10" s="22"/>
+      <c r="AY10" s="22" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -3191,7 +2976,7 @@
       </c>
       <c r="N11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(N5), ISBLANK(N6), ISBLANK(N7), ISBLANK(N8), ISBLANK(N9), ISBLANK(N10))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="O11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(O5), ISBLANK(O6), ISBLANK(O7), ISBLANK(O8), ISBLANK(O9), ISBLANK(O10))), "Yes", "No")</f>
@@ -3199,11 +2984,11 @@
       </c>
       <c r="P11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(P5), ISBLANK(P6), ISBLANK(P7), ISBLANK(P8), ISBLANK(P9), ISBLANK(P10))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="Q11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(Q5), ISBLANK(Q6), ISBLANK(Q7), ISBLANK(Q8), ISBLANK(Q9), ISBLANK(Q10))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="R11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(R5), ISBLANK(R6), ISBLANK(R7), ISBLANK(R8), ISBLANK(R9), ISBLANK(R10))), "Yes", "No")</f>
@@ -3211,11 +2996,11 @@
       </c>
       <c r="S11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(S5), ISBLANK(S6), ISBLANK(S7), ISBLANK(S8), ISBLANK(S9), ISBLANK(S10))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="T11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(T5), ISBLANK(T6), ISBLANK(T7), ISBLANK(T8), ISBLANK(T9), ISBLANK(T10))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="U11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(U5), ISBLANK(U6), ISBLANK(U7), ISBLANK(U8), ISBLANK(U9), ISBLANK(U10))), "Yes", "No")</f>
@@ -3227,19 +3012,19 @@
       </c>
       <c r="W11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(W5), ISBLANK(W6), ISBLANK(W7), ISBLANK(W8), ISBLANK(W9), ISBLANK(W10))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="X11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(X5), ISBLANK(X6), ISBLANK(X7), ISBLANK(X8), ISBLANK(X9), ISBLANK(X10))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="Y11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(Y5), ISBLANK(Y6), ISBLANK(Y7), ISBLANK(Y8), ISBLANK(Y9), ISBLANK(Y10))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="Z11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(Z5), ISBLANK(Z6), ISBLANK(Z7), ISBLANK(Z8), ISBLANK(Z9), ISBLANK(Z10))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AA11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AA5), ISBLANK(AA6), ISBLANK(AA7), ISBLANK(AA8), ISBLANK(AA9), ISBLANK(AA10))), "Yes", "No")</f>
@@ -3247,7 +3032,7 @@
       </c>
       <c r="AB11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AB5), ISBLANK(AB6), ISBLANK(AB7), ISBLANK(AB8), ISBLANK(AB9), ISBLANK(AB10))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AC11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AC5), ISBLANK(AC6), ISBLANK(AC7), ISBLANK(AC8), ISBLANK(AC9), ISBLANK(AC10))), "Yes", "No")</f>
@@ -3255,7 +3040,7 @@
       </c>
       <c r="AD11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AD5), ISBLANK(AD6), ISBLANK(AD7), ISBLANK(AD8), ISBLANK(AD9), ISBLANK(AD10))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AE11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AE5), ISBLANK(AE6), ISBLANK(AE7), ISBLANK(AE8), ISBLANK(AE9), ISBLANK(AE10))), "Yes", "No")</f>
@@ -3275,7 +3060,7 @@
       </c>
       <c r="AI11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AI5), ISBLANK(AI6), ISBLANK(AI7), ISBLANK(AI8), ISBLANK(AI9), ISBLANK(AI10))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AJ11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AJ5), ISBLANK(AJ6), ISBLANK(AJ7), ISBLANK(AJ8), ISBLANK(AJ9), ISBLANK(AJ10))), "Yes", "No")</f>
@@ -3283,7 +3068,7 @@
       </c>
       <c r="AK11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AK5), ISBLANK(AK6), ISBLANK(AK7), ISBLANK(AK8), ISBLANK(AK9), ISBLANK(AK10))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AL11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AL5), ISBLANK(AL6), ISBLANK(AL7), ISBLANK(AL8), ISBLANK(AL9), ISBLANK(AL10))), "Yes", "No")</f>
@@ -3291,7 +3076,7 @@
       </c>
       <c r="AM11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AM5), ISBLANK(AM6), ISBLANK(AM7), ISBLANK(AM8), ISBLANK(AM9), ISBLANK(AM10))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AN11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AN5), ISBLANK(AN6), ISBLANK(AN7), ISBLANK(AN8), ISBLANK(AN9), ISBLANK(AN10))), "Yes", "No")</f>
@@ -3299,7 +3084,7 @@
       </c>
       <c r="AO11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AO5), ISBLANK(AO6), ISBLANK(AO7), ISBLANK(AO8), ISBLANK(AO9), ISBLANK(AO10))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AP11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AP5), ISBLANK(AP6), ISBLANK(AP7), ISBLANK(AP8), ISBLANK(AP9), ISBLANK(AP10))), "Yes", "No")</f>
@@ -3307,7 +3092,7 @@
       </c>
       <c r="AQ11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AQ5), ISBLANK(AQ6), ISBLANK(AQ7), ISBLANK(AQ8), ISBLANK(AQ9), ISBLANK(AQ10))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AR11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AR5), ISBLANK(AR6), ISBLANK(AR7), ISBLANK(AR8), ISBLANK(AR9), ISBLANK(AR10))), "Yes", "No")</f>
@@ -3315,7 +3100,7 @@
       </c>
       <c r="AS11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AS5), ISBLANK(AS6), ISBLANK(AS7), ISBLANK(AS8), ISBLANK(AS9), ISBLANK(AS10))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AT11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AT5), ISBLANK(AT6), ISBLANK(AT7), ISBLANK(AT8), ISBLANK(AT9), ISBLANK(AT10))), "Yes", "No")</f>
@@ -3331,7 +3116,7 @@
       </c>
       <c r="AW11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AW5), ISBLANK(AW6), ISBLANK(AW7), ISBLANK(AW8), ISBLANK(AW9), ISBLANK(AW10))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AX11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AX5), ISBLANK(AX6), ISBLANK(AX7), ISBLANK(AX8), ISBLANK(AX9), ISBLANK(AX10))), "Yes", "No")</f>
@@ -3339,7 +3124,7 @@
       </c>
       <c r="AY11" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AY5), ISBLANK(AY6), ISBLANK(AY7), ISBLANK(AY8), ISBLANK(AY9), ISBLANK(AY10))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3913,7 +3698,7 @@
       <c r="N16" s="11"/>
       <c r="O16" s="12"/>
       <c r="P16" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Q16" s="11"/>
       <c r="R16" s="11" t="s">
@@ -3938,17 +3723,19 @@
       <c r="AC16" s="11"/>
       <c r="AD16" s="11"/>
       <c r="AE16" s="11"/>
-      <c r="AF16" s="11"/>
+      <c r="AF16" s="11" t="s">
+        <v>127</v>
+      </c>
       <c r="AG16" s="11"/>
       <c r="AH16" s="11" t="s">
         <v>121</v>
       </c>
       <c r="AI16" s="12"/>
       <c r="AJ16" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="AK16" s="12" t="s">
         <v>127</v>
-      </c>
-      <c r="AK16" s="12" t="s">
-        <v>128</v>
       </c>
       <c r="AL16" s="11"/>
       <c r="AM16" s="12"/>
@@ -4194,48 +3981,76 @@
         <v>70</v>
       </c>
       <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
+      <c r="C21" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
+      <c r="E21" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="G21" s="21"/>
       <c r="H21" s="20"/>
       <c r="I21" s="21"/>
-      <c r="J21" s="20"/>
+      <c r="J21" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="21"/>
+      <c r="N21" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="O21" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="P21" s="20"/>
-      <c r="Q21" s="20"/>
+      <c r="Q21" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="R21" s="20"/>
-      <c r="S21" s="20"/>
+      <c r="S21" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="T21" s="20"/>
       <c r="U21" s="20"/>
       <c r="V21" s="20"/>
       <c r="W21" s="20"/>
       <c r="X21" s="20"/>
       <c r="Y21" s="20"/>
-      <c r="Z21" s="20"/>
+      <c r="Z21" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AA21" s="20"/>
       <c r="AB21" s="20"/>
-      <c r="AC21" s="20"/>
+      <c r="AC21" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AD21" s="20"/>
       <c r="AE21" s="20"/>
       <c r="AF21" s="20"/>
-      <c r="AG21" s="20"/>
+      <c r="AG21" s="21"/>
       <c r="AH21" s="20"/>
-      <c r="AI21" s="21"/>
+      <c r="AI21" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AJ21" s="20"/>
       <c r="AK21" s="21"/>
-      <c r="AL21" s="20"/>
+      <c r="AL21" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AM21" s="21"/>
       <c r="AN21" s="20"/>
       <c r="AO21" s="21"/>
       <c r="AP21" s="20"/>
-      <c r="AQ21" s="21"/>
-      <c r="AR21" s="20"/>
+      <c r="AQ21" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="AR21" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AS21" s="21"/>
       <c r="AT21" s="20"/>
       <c r="AU21" s="21"/>
@@ -4254,7 +4069,7 @@
       </c>
       <c r="C22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(C16), ISBLANK(C17), ISBLANK(C18), ISBLANK(C19), ISBLANK(C20), ISBLANK(C21))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="D22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(D16), ISBLANK(D17), ISBLANK(D18), ISBLANK(D19), ISBLANK(D20), ISBLANK(D21))), "Yes", "No")</f>
@@ -4262,11 +4077,11 @@
       </c>
       <c r="E22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(E16), ISBLANK(E17), ISBLANK(E18), ISBLANK(E19), ISBLANK(E20), ISBLANK(E21))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="F22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(F16), ISBLANK(F17), ISBLANK(F18), ISBLANK(F19), ISBLANK(F20), ISBLANK(F21))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="G22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(G16), ISBLANK(G17), ISBLANK(G18), ISBLANK(G19), ISBLANK(G20), ISBLANK(G21))), "Yes", "No")</f>
@@ -4282,7 +4097,7 @@
       </c>
       <c r="J22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(J16), ISBLANK(J17), ISBLANK(J18), ISBLANK(J19), ISBLANK(J20), ISBLANK(J21))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="K22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(K16), ISBLANK(K17), ISBLANK(K18), ISBLANK(K19), ISBLANK(K20), ISBLANK(K21))), "Yes", "No")</f>
@@ -4298,11 +4113,11 @@
       </c>
       <c r="N22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(N16), ISBLANK(N17), ISBLANK(N18), ISBLANK(N19), ISBLANK(N20), ISBLANK(N21))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="O22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(O16), ISBLANK(O17), ISBLANK(O18), ISBLANK(O19), ISBLANK(O20), ISBLANK(O21))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="P22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(P16), ISBLANK(P17), ISBLANK(P18), ISBLANK(P19), ISBLANK(P20), ISBLANK(P21))), "Yes", "No")</f>
@@ -4310,7 +4125,7 @@
       </c>
       <c r="Q22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(Q16), ISBLANK(Q17), ISBLANK(Q18), ISBLANK(Q19), ISBLANK(Q20), ISBLANK(Q21))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="R22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(R16), ISBLANK(R17), ISBLANK(R18), ISBLANK(R19), ISBLANK(R20), ISBLANK(R21))), "Yes", "No")</f>
@@ -4318,7 +4133,7 @@
       </c>
       <c r="S22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(S16), ISBLANK(S17), ISBLANK(S18), ISBLANK(S19), ISBLANK(S20), ISBLANK(S21))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="T22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(T16), ISBLANK(T17), ISBLANK(T18), ISBLANK(T19), ISBLANK(T20), ISBLANK(T21))), "Yes", "No")</f>
@@ -4346,7 +4161,7 @@
       </c>
       <c r="Z22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(Z16), ISBLANK(Z17), ISBLANK(Z18), ISBLANK(Z19), ISBLANK(Z20), ISBLANK(Z21))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AA22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AA16), ISBLANK(AA17), ISBLANK(AA18), ISBLANK(AA19), ISBLANK(AA20), ISBLANK(AA21))), "Yes", "No")</f>
@@ -4358,7 +4173,7 @@
       </c>
       <c r="AC22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AC16), ISBLANK(AC17), ISBLANK(AC18), ISBLANK(AC19), ISBLANK(AC20), ISBLANK(AC21))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AD22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AD16), ISBLANK(AD17), ISBLANK(AD18), ISBLANK(AD19), ISBLANK(AD20), ISBLANK(AD21))), "Yes", "No")</f>
@@ -4370,7 +4185,7 @@
       </c>
       <c r="AF22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AF16), ISBLANK(AF17), ISBLANK(AF18), ISBLANK(AF19), ISBLANK(AF20), ISBLANK(AF21))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AG22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AG16), ISBLANK(AG17), ISBLANK(AG18), ISBLANK(AG19), ISBLANK(AG20), ISBLANK(AG21))), "Yes", "No")</f>
@@ -4382,7 +4197,7 @@
       </c>
       <c r="AI22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AI16), ISBLANK(AI17), ISBLANK(AI18), ISBLANK(AI19), ISBLANK(AI20), ISBLANK(AI21))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AJ22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AJ16), ISBLANK(AJ17), ISBLANK(AJ18), ISBLANK(AJ19), ISBLANK(AJ20), ISBLANK(AJ21))), "Yes", "No")</f>
@@ -4394,7 +4209,7 @@
       </c>
       <c r="AL22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AL16), ISBLANK(AL17), ISBLANK(AL18), ISBLANK(AL19), ISBLANK(AL20), ISBLANK(AL21))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AM22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AM16), ISBLANK(AM17), ISBLANK(AM18), ISBLANK(AM19), ISBLANK(AM20), ISBLANK(AM21))), "Yes", "No")</f>
@@ -4414,11 +4229,11 @@
       </c>
       <c r="AQ22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AQ16), ISBLANK(AQ17), ISBLANK(AQ18), ISBLANK(AQ19), ISBLANK(AQ20), ISBLANK(AQ21))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AR22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AR16), ISBLANK(AR17), ISBLANK(AR18), ISBLANK(AR19), ISBLANK(AR20), ISBLANK(AR21))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AS22" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AS16), ISBLANK(AS17), ISBLANK(AS18), ISBLANK(AS19), ISBLANK(AS20), ISBLANK(AS21))), "Yes", "No")</f>
@@ -5066,7 +4881,7 @@
       <c r="AD27" s="11"/>
       <c r="AE27" s="11"/>
       <c r="AF27" s="11" t="s">
-        <v>129</v>
+        <v>182</v>
       </c>
       <c r="AG27" s="11"/>
       <c r="AH27" s="11" t="s">
@@ -5074,23 +4889,27 @@
       </c>
       <c r="AI27" s="12"/>
       <c r="AJ27" s="31" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AK27" s="12"/>
       <c r="AL27" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AM27" s="12"/>
-      <c r="AN27" s="11"/>
+      <c r="AN27" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="AO27" s="12"/>
-      <c r="AP27" s="11"/>
+      <c r="AP27" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="AQ27" s="12"/>
       <c r="AR27" s="11"/>
       <c r="AS27" s="12"/>
       <c r="AT27" s="11"/>
       <c r="AU27" s="12"/>
       <c r="AV27" s="11" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AW27" s="12"/>
       <c r="AX27" s="11"/>
@@ -5323,43 +5142,77 @@
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
       <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
+      <c r="E32" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="F32" s="20"/>
       <c r="G32" s="21"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="21"/>
+      <c r="H32" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="I32" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
+      <c r="K32" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="L32" s="20"/>
-      <c r="M32" s="20"/>
+      <c r="M32" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="N32" s="20"/>
       <c r="O32" s="21"/>
       <c r="P32" s="20"/>
-      <c r="Q32" s="20"/>
+      <c r="Q32" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="R32" s="20"/>
-      <c r="S32" s="20"/>
+      <c r="S32" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="T32" s="20"/>
-      <c r="U32" s="20"/>
+      <c r="U32" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="V32" s="20"/>
-      <c r="W32" s="20"/>
+      <c r="W32" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="X32" s="20"/>
-      <c r="Y32" s="20"/>
+      <c r="Y32" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="Z32" s="20"/>
-      <c r="AA32" s="20"/>
+      <c r="AA32" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AB32" s="20"/>
-      <c r="AC32" s="20"/>
+      <c r="AC32" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AD32" s="20"/>
       <c r="AE32" s="20"/>
       <c r="AF32" s="20"/>
-      <c r="AG32" s="20"/>
+      <c r="AG32" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AH32" s="20"/>
-      <c r="AI32" s="21"/>
+      <c r="AI32" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AJ32" s="20"/>
-      <c r="AK32" s="21"/>
+      <c r="AK32" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AL32" s="20"/>
-      <c r="AM32" s="21"/>
+      <c r="AM32" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AN32" s="20"/>
-      <c r="AO32" s="21"/>
+      <c r="AO32" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AP32" s="20"/>
       <c r="AQ32" s="21"/>
       <c r="AR32" s="20"/>
@@ -5367,7 +5220,9 @@
       <c r="AT32" s="20"/>
       <c r="AU32" s="21"/>
       <c r="AV32" s="20"/>
-      <c r="AW32" s="21"/>
+      <c r="AW32" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AX32" s="20"/>
       <c r="AY32" s="22"/>
     </row>
@@ -5389,7 +5244,7 @@
       </c>
       <c r="E33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(E27), ISBLANK(E28), ISBLANK(E29), ISBLANK(E30), ISBLANK(E31), ISBLANK(E32))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="F33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(F27), ISBLANK(F28), ISBLANK(F29), ISBLANK(F30), ISBLANK(F31), ISBLANK(F32))), "Yes", "No")</f>
@@ -5401,11 +5256,11 @@
       </c>
       <c r="H33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(H27), ISBLANK(H28), ISBLANK(H29), ISBLANK(H30), ISBLANK(H31), ISBLANK(H32))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="I33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(I27), ISBLANK(I28), ISBLANK(I29), ISBLANK(I30), ISBLANK(I31), ISBLANK(I32))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="J33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(J27), ISBLANK(J28), ISBLANK(J29), ISBLANK(J30), ISBLANK(J31), ISBLANK(J32))), "Yes", "No")</f>
@@ -5413,7 +5268,7 @@
       </c>
       <c r="K33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(K27), ISBLANK(K28), ISBLANK(K29), ISBLANK(K30), ISBLANK(K31), ISBLANK(K32))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="L33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(L27), ISBLANK(L28), ISBLANK(L29), ISBLANK(L30), ISBLANK(L31), ISBLANK(L32))), "Yes", "No")</f>
@@ -5421,7 +5276,7 @@
       </c>
       <c r="M33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(M27), ISBLANK(M28), ISBLANK(M29), ISBLANK(M30), ISBLANK(M31), ISBLANK(M32))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="N33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(N27), ISBLANK(N28), ISBLANK(N29), ISBLANK(N30), ISBLANK(N31), ISBLANK(N32))), "Yes", "No")</f>
@@ -5437,7 +5292,7 @@
       </c>
       <c r="Q33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(Q27), ISBLANK(Q28), ISBLANK(Q29), ISBLANK(Q30), ISBLANK(Q31), ISBLANK(Q32))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="R33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(R27), ISBLANK(R28), ISBLANK(R29), ISBLANK(R30), ISBLANK(R31), ISBLANK(R32))), "Yes", "No")</f>
@@ -5445,7 +5300,7 @@
       </c>
       <c r="S33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(S27), ISBLANK(S28), ISBLANK(S29), ISBLANK(S30), ISBLANK(S31), ISBLANK(S32))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="T33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(T27), ISBLANK(T28), ISBLANK(T29), ISBLANK(T30), ISBLANK(T31), ISBLANK(T32))), "Yes", "No")</f>
@@ -5453,7 +5308,7 @@
       </c>
       <c r="U33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(U27), ISBLANK(U28), ISBLANK(U29), ISBLANK(U30), ISBLANK(U31), ISBLANK(U32))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="V33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(V27), ISBLANK(V28), ISBLANK(V29), ISBLANK(V30), ISBLANK(V31), ISBLANK(V32))), "Yes", "No")</f>
@@ -5461,7 +5316,7 @@
       </c>
       <c r="W33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(W27), ISBLANK(W28), ISBLANK(W29), ISBLANK(W30), ISBLANK(W31), ISBLANK(W32))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="X33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(X27), ISBLANK(X28), ISBLANK(X29), ISBLANK(X30), ISBLANK(X31), ISBLANK(X32))), "Yes", "No")</f>
@@ -5469,7 +5324,7 @@
       </c>
       <c r="Y33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(Y27), ISBLANK(Y28), ISBLANK(Y29), ISBLANK(Y30), ISBLANK(Y31), ISBLANK(Y32))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="Z33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(Z27), ISBLANK(Z28), ISBLANK(Z29), ISBLANK(Z30), ISBLANK(Z31), ISBLANK(Z32))), "Yes", "No")</f>
@@ -5477,7 +5332,7 @@
       </c>
       <c r="AA33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AA27), ISBLANK(AA28), ISBLANK(AA29), ISBLANK(AA30), ISBLANK(AA31), ISBLANK(AA32))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AB33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AB27), ISBLANK(AB28), ISBLANK(AB29), ISBLANK(AB30), ISBLANK(AB31), ISBLANK(AB32))), "Yes", "No")</f>
@@ -5485,7 +5340,7 @@
       </c>
       <c r="AC33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AC27), ISBLANK(AC28), ISBLANK(AC29), ISBLANK(AC30), ISBLANK(AC31), ISBLANK(AC32))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AD33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AD27), ISBLANK(AD28), ISBLANK(AD29), ISBLANK(AD30), ISBLANK(AD31), ISBLANK(AD32))), "Yes", "No")</f>
@@ -5501,7 +5356,7 @@
       </c>
       <c r="AG33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AG27), ISBLANK(AG28), ISBLANK(AG29), ISBLANK(AG30), ISBLANK(AG31), ISBLANK(AG32))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AH33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AH27), ISBLANK(AH28), ISBLANK(AH29), ISBLANK(AH30), ISBLANK(AH31), ISBLANK(AH32))), "Yes", "No")</f>
@@ -5509,7 +5364,7 @@
       </c>
       <c r="AI33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AI27), ISBLANK(AI28), ISBLANK(AI29), ISBLANK(AI30), ISBLANK(AI31), ISBLANK(AI32))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AJ33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AJ27), ISBLANK(AJ28), ISBLANK(AJ29), ISBLANK(AJ30), ISBLANK(AJ31), ISBLANK(AJ32))), "Yes", "No")</f>
@@ -5517,7 +5372,7 @@
       </c>
       <c r="AK33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AK27), ISBLANK(AK28), ISBLANK(AK29), ISBLANK(AK30), ISBLANK(AK31), ISBLANK(AK32))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AL33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AL27), ISBLANK(AL28), ISBLANK(AL29), ISBLANK(AL30), ISBLANK(AL31), ISBLANK(AL32))), "Yes", "No")</f>
@@ -5525,19 +5380,19 @@
       </c>
       <c r="AM33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AM27), ISBLANK(AM28), ISBLANK(AM29), ISBLANK(AM30), ISBLANK(AM31), ISBLANK(AM32))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AN33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AN27), ISBLANK(AN28), ISBLANK(AN29), ISBLANK(AN30), ISBLANK(AN31), ISBLANK(AN32))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AO33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AO27), ISBLANK(AO28), ISBLANK(AO29), ISBLANK(AO30), ISBLANK(AO31), ISBLANK(AO32))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AP33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AP27), ISBLANK(AP28), ISBLANK(AP29), ISBLANK(AP30), ISBLANK(AP31), ISBLANK(AP32))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AQ33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AQ27), ISBLANK(AQ28), ISBLANK(AQ29), ISBLANK(AQ30), ISBLANK(AQ31), ISBLANK(AQ32))), "Yes", "No")</f>
@@ -5565,7 +5420,7 @@
       </c>
       <c r="AW33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AW27), ISBLANK(AW28), ISBLANK(AW29), ISBLANK(AW30), ISBLANK(AW31), ISBLANK(AW32))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="AX33" s="23" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AX27), ISBLANK(AX28), ISBLANK(AX29), ISBLANK(AX30), ISBLANK(AX31), ISBLANK(AX32))), "Yes", "No")</f>
@@ -5736,119 +5591,119 @@
         <v>1</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="6"/>
       <c r="J35" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="L35" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="N35" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="O35" s="6"/>
       <c r="P35" s="5"/>
       <c r="Q35" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="R35" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="S35" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="T35" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="U35" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="V35" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="W35" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="X35" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="Y35" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="Z35" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AA35" s="5"/>
       <c r="AB35" s="5"/>
       <c r="AC35" s="5"/>
       <c r="AD35" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AE35" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AF35" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AG35" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AH35" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AI35" s="6" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AJ35" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AK35" s="6" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AL35" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="AM35" s="6" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AN35" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AO35" s="6" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AP35" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="AQ35" s="6" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AR35" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AS35" s="6"/>
       <c r="AT35" s="5"/>
@@ -5857,7 +5712,7 @@
       <c r="AW35" s="6"/>
       <c r="AX35" s="5"/>
       <c r="AY35" s="25" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6128,21 +5983,21 @@
       <c r="O38" s="33"/>
       <c r="P38" s="32"/>
       <c r="Q38" s="32" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="R38" s="32"/>
       <c r="S38" s="32" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="T38" s="32" t="s">
         <v>129</v>
       </c>
       <c r="U38" s="32"/>
       <c r="V38" s="32" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="W38" s="32" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="X38" s="32"/>
       <c r="Y38" s="32"/>
@@ -6151,7 +6006,7 @@
       <c r="AB38" s="32"/>
       <c r="AC38" s="32"/>
       <c r="AD38" s="32" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AE38" s="32"/>
       <c r="AF38" s="32" t="s">
@@ -6159,7 +6014,7 @@
       </c>
       <c r="AG38" s="32"/>
       <c r="AH38" s="32" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AI38" s="33"/>
       <c r="AJ38" s="32" t="s">
@@ -6178,7 +6033,7 @@
       <c r="AQ38" s="33"/>
       <c r="AR38" s="32"/>
       <c r="AS38" s="33" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AT38" s="32"/>
       <c r="AU38" s="33"/>
@@ -6412,325 +6267,362 @@
         <v>70</v>
       </c>
       <c r="B43" s="41"/>
-      <c r="C43" s="41"/>
+      <c r="C43" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="D43" s="41"/>
-      <c r="E43" s="41"/>
+      <c r="E43" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="F43" s="41"/>
-      <c r="G43" s="42"/>
+      <c r="G43" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="H43" s="41"/>
       <c r="I43" s="42"/>
       <c r="J43" s="41"/>
-      <c r="K43" s="41"/>
+      <c r="K43" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="L43" s="41"/>
       <c r="M43" s="41"/>
       <c r="N43" s="41"/>
       <c r="O43" s="42"/>
       <c r="P43" s="41"/>
       <c r="Q43" s="41"/>
-      <c r="R43" s="41"/>
+      <c r="R43" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="S43" s="41"/>
       <c r="T43" s="41"/>
-      <c r="U43" s="41"/>
+      <c r="U43" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="V43" s="41"/>
       <c r="W43" s="41"/>
-      <c r="X43" s="41"/>
+      <c r="X43" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="Y43" s="41"/>
       <c r="Z43" s="41"/>
       <c r="AA43" s="41"/>
       <c r="AB43" s="41"/>
       <c r="AC43" s="41"/>
       <c r="AD43" s="41"/>
-      <c r="AE43" s="41"/>
+      <c r="AE43" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AF43" s="41"/>
-      <c r="AG43" s="41"/>
+      <c r="AG43" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AH43" s="41"/>
-      <c r="AI43" s="42"/>
+      <c r="AI43" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AJ43" s="41"/>
-      <c r="AK43" s="42"/>
-      <c r="AL43" s="41"/>
+      <c r="AK43" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL43" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AM43" s="42"/>
-      <c r="AN43" s="41"/>
-      <c r="AO43" s="42"/>
+      <c r="AN43" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO43" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AP43" s="41"/>
-      <c r="AQ43" s="42"/>
-      <c r="AR43" s="41"/>
+      <c r="AQ43" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="AR43" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AS43" s="42"/>
-      <c r="AT43" s="41"/>
-      <c r="AU43" s="42"/>
+      <c r="AT43" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="AU43" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="AV43" s="41"/>
       <c r="AW43" s="42"/>
       <c r="AX43" s="41"/>
-      <c r="AY43" s="43"/>
+      <c r="AY43" s="22" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B44" s="44" t="str">
+      <c r="B44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(B38), ISBLANK(B39), ISBLANK(B40), ISBLANK(B41), ISBLANK(B42), ISBLANK(B43))), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="C44" s="44" t="str">
+      <c r="C44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(C38), ISBLANK(C39), ISBLANK(C40), ISBLANK(C41), ISBLANK(C42), ISBLANK(C43))), "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="D44" s="44" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="D44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(D38), ISBLANK(D39), ISBLANK(D40), ISBLANK(D41), ISBLANK(D42), ISBLANK(D43))), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="E44" s="44" t="str">
+      <c r="E44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(E38), ISBLANK(E39), ISBLANK(E40), ISBLANK(E41), ISBLANK(E42), ISBLANK(E43))), "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="F44" s="44" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="F44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(F38), ISBLANK(F39), ISBLANK(F40), ISBLANK(F41), ISBLANK(F42), ISBLANK(F43))), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="G44" s="44" t="str">
+      <c r="G44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(G38), ISBLANK(G39), ISBLANK(G40), ISBLANK(G41), ISBLANK(G42), ISBLANK(G43))), "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="H44" s="44" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="H44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(H38), ISBLANK(H39), ISBLANK(H40), ISBLANK(H41), ISBLANK(H42), ISBLANK(H43))), "Yes", "No")</f>
         <v>No</v>
       </c>
-      <c r="I44" s="44" t="str">
+      <c r="I44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(I38), ISBLANK(I39), ISBLANK(I40), ISBLANK(I41), ISBLANK(I42), ISBLANK(I43))), "Yes", "No")</f>
         <v>No</v>
       </c>
-      <c r="J44" s="44" t="str">
+      <c r="J44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(J38), ISBLANK(J39), ISBLANK(J40), ISBLANK(J41), ISBLANK(J42), ISBLANK(J43))), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="K44" s="44" t="str">
+      <c r="K44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(K38), ISBLANK(K39), ISBLANK(K40), ISBLANK(K41), ISBLANK(K42), ISBLANK(K43))), "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="L44" s="44" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="L44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(L38), ISBLANK(L39), ISBLANK(L40), ISBLANK(L41), ISBLANK(L42), ISBLANK(L43))), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="M44" s="44" t="str">
+      <c r="M44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(M38), ISBLANK(M39), ISBLANK(M40), ISBLANK(M41), ISBLANK(M42), ISBLANK(M43))), "Yes", "No")</f>
         <v>No</v>
       </c>
-      <c r="N44" s="44" t="str">
+      <c r="N44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(N38), ISBLANK(N39), ISBLANK(N40), ISBLANK(N41), ISBLANK(N42), ISBLANK(N43))), "Yes", "No")</f>
         <v>No</v>
       </c>
-      <c r="O44" s="44" t="str">
+      <c r="O44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(O38), ISBLANK(O39), ISBLANK(O40), ISBLANK(O41), ISBLANK(O42), ISBLANK(O43))), "Yes", "No")</f>
         <v>No</v>
       </c>
-      <c r="P44" s="44" t="str">
+      <c r="P44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(P38), ISBLANK(P39), ISBLANK(P40), ISBLANK(P41), ISBLANK(P42), ISBLANK(P43))), "Yes", "No")</f>
         <v>No</v>
       </c>
-      <c r="Q44" s="44" t="str">
+      <c r="Q44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(Q38), ISBLANK(Q39), ISBLANK(Q40), ISBLANK(Q41), ISBLANK(Q42), ISBLANK(Q43))), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="R44" s="44" t="str">
+      <c r="R44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(R38), ISBLANK(R39), ISBLANK(R40), ISBLANK(R41), ISBLANK(R42), ISBLANK(R43))), "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="S44" s="44" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="S44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(S38), ISBLANK(S39), ISBLANK(S40), ISBLANK(S41), ISBLANK(S42), ISBLANK(S43))), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="T44" s="44" t="str">
+      <c r="T44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(T38), ISBLANK(T39), ISBLANK(T40), ISBLANK(T41), ISBLANK(T42), ISBLANK(T43))), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="U44" s="44" t="str">
+      <c r="U44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(U38), ISBLANK(U39), ISBLANK(U40), ISBLANK(U41), ISBLANK(U42), ISBLANK(U43))), "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="V44" s="44" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="V44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(V38), ISBLANK(V39), ISBLANK(V40), ISBLANK(V41), ISBLANK(V42), ISBLANK(V43))), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="W44" s="44" t="str">
+      <c r="W44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(W38), ISBLANK(W39), ISBLANK(W40), ISBLANK(W41), ISBLANK(W42), ISBLANK(W43))), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="X44" s="44" t="str">
+      <c r="X44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(X38), ISBLANK(X39), ISBLANK(X40), ISBLANK(X41), ISBLANK(X42), ISBLANK(X43))), "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="Y44" s="44" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="Y44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(Y38), ISBLANK(Y39), ISBLANK(Y40), ISBLANK(Y41), ISBLANK(Y42), ISBLANK(Y43))), "Yes", "No")</f>
         <v>No</v>
       </c>
-      <c r="Z44" s="44" t="str">
+      <c r="Z44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(Z38), ISBLANK(Z39), ISBLANK(Z40), ISBLANK(Z41), ISBLANK(Z42), ISBLANK(Z43))), "Yes", "No")</f>
         <v>No</v>
       </c>
-      <c r="AA44" s="44" t="str">
+      <c r="AA44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AA38), ISBLANK(AA39), ISBLANK(AA40), ISBLANK(AA41), ISBLANK(AA42), ISBLANK(AA43))), "Yes", "No")</f>
         <v>No</v>
       </c>
-      <c r="AB44" s="44" t="str">
+      <c r="AB44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AB38), ISBLANK(AB39), ISBLANK(AB40), ISBLANK(AB41), ISBLANK(AB42), ISBLANK(AB43))), "Yes", "No")</f>
         <v>No</v>
       </c>
-      <c r="AC44" s="44" t="str">
+      <c r="AC44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AC38), ISBLANK(AC39), ISBLANK(AC40), ISBLANK(AC41), ISBLANK(AC42), ISBLANK(AC43))), "Yes", "No")</f>
         <v>No</v>
       </c>
-      <c r="AD44" s="44" t="str">
+      <c r="AD44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AD38), ISBLANK(AD39), ISBLANK(AD40), ISBLANK(AD41), ISBLANK(AD42), ISBLANK(AD43))), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="AE44" s="44" t="str">
+      <c r="AE44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AE38), ISBLANK(AE39), ISBLANK(AE40), ISBLANK(AE41), ISBLANK(AE42), ISBLANK(AE43))), "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="AF44" s="44" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="AF44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AF38), ISBLANK(AF39), ISBLANK(AF40), ISBLANK(AF41), ISBLANK(AF42), ISBLANK(AF43))), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="AG44" s="44" t="str">
+      <c r="AG44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AG38), ISBLANK(AG39), ISBLANK(AG40), ISBLANK(AG41), ISBLANK(AG42), ISBLANK(AG43))), "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="AH44" s="44" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="AH44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AH38), ISBLANK(AH39), ISBLANK(AH40), ISBLANK(AH41), ISBLANK(AH42), ISBLANK(AH43))), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="AI44" s="44" t="str">
+      <c r="AI44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AI38), ISBLANK(AI39), ISBLANK(AI40), ISBLANK(AI41), ISBLANK(AI42), ISBLANK(AI43))), "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="AJ44" s="44" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="AJ44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AJ38), ISBLANK(AJ39), ISBLANK(AJ40), ISBLANK(AJ41), ISBLANK(AJ42), ISBLANK(AJ43))), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="AK44" s="44" t="str">
+      <c r="AK44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AK38), ISBLANK(AK39), ISBLANK(AK40), ISBLANK(AK41), ISBLANK(AK42), ISBLANK(AK43))), "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="AL44" s="44" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="AL44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AL38), ISBLANK(AL39), ISBLANK(AL40), ISBLANK(AL41), ISBLANK(AL42), ISBLANK(AL43))), "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="AM44" s="44" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="AM44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AM38), ISBLANK(AM39), ISBLANK(AM40), ISBLANK(AM41), ISBLANK(AM42), ISBLANK(AM43))), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="AN44" s="44" t="str">
+      <c r="AN44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AN38), ISBLANK(AN39), ISBLANK(AN40), ISBLANK(AN41), ISBLANK(AN42), ISBLANK(AN43))), "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="AO44" s="44" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="AO44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AO38), ISBLANK(AO39), ISBLANK(AO40), ISBLANK(AO41), ISBLANK(AO42), ISBLANK(AO43))), "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="AP44" s="44" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="AP44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AP38), ISBLANK(AP39), ISBLANK(AP40), ISBLANK(AP41), ISBLANK(AP42), ISBLANK(AP43))), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="AQ44" s="44" t="str">
+      <c r="AQ44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AQ38), ISBLANK(AQ39), ISBLANK(AQ40), ISBLANK(AQ41), ISBLANK(AQ42), ISBLANK(AQ43))), "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="AR44" s="44" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="AR44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AR38), ISBLANK(AR39), ISBLANK(AR40), ISBLANK(AR41), ISBLANK(AR42), ISBLANK(AR43))), "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="AS44" s="44" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="AS44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AS38), ISBLANK(AS39), ISBLANK(AS40), ISBLANK(AS41), ISBLANK(AS42), ISBLANK(AS43))), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-      <c r="AT44" s="44" t="str">
+      <c r="AT44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AT38), ISBLANK(AT39), ISBLANK(AT40), ISBLANK(AT41), ISBLANK(AT42), ISBLANK(AT43))), "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="AU44" s="44" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="AU44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AU38), ISBLANK(AU39), ISBLANK(AU40), ISBLANK(AU41), ISBLANK(AU42), ISBLANK(AU43))), "Yes", "No")</f>
-        <v>No</v>
-      </c>
-      <c r="AV44" s="44" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="AV44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AV38), ISBLANK(AV39), ISBLANK(AV40), ISBLANK(AV41), ISBLANK(AV42), ISBLANK(AV43))), "Yes", "No")</f>
         <v>No</v>
       </c>
-      <c r="AW44" s="44" t="str">
+      <c r="AW44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AW38), ISBLANK(AW39), ISBLANK(AW40), ISBLANK(AW41), ISBLANK(AW42), ISBLANK(AW43))), "Yes", "No")</f>
         <v>No</v>
       </c>
-      <c r="AX44" s="44" t="str">
+      <c r="AX44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AX38), ISBLANK(AX39), ISBLANK(AX40), ISBLANK(AX41), ISBLANK(AX42), ISBLANK(AX43))), "Yes", "No")</f>
         <v>No</v>
       </c>
-      <c r="AY44" s="44" t="str">
+      <c r="AY44" s="43" t="str">
         <f aca="false">IF(NOT(AND(ISBLANK(AY38), ISBLANK(AY39), ISBLANK(AY40), ISBLANK(AY41), ISBLANK(AY42), ISBLANK(AY43))), "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="45" t="s">
-        <v>226</v>
-      </c>
-      <c r="B46" s="46" t="s">
-        <v>227</v>
-      </c>
-      <c r="D46" s="45" t="s">
+      <c r="A46" s="44" t="s">
         <v>228</v>
       </c>
-      <c r="E46" s="46" t="n">
-        <f aca="false">SUM(E47,E48)</f>
+      <c r="B46" s="45" t="s">
+        <v>229</v>
+      </c>
+      <c r="D46" s="44" t="s">
+        <v>230</v>
+      </c>
+      <c r="E46" s="45" t="n">
+        <f aca="false">COUNTIF((B2:AY2~ B13:AY13~ B24:AY24~ B35:AY35), "")</f>
         <v>38</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="J46" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="47" t="s">
+      <c r="A47" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="B47" s="48" t="n">
+      <c r="B47" s="47" t="n">
         <f aca="false">COUNTIF((B3:AY4~B14:AY15~B25:AY26~B36:AY37),"Normal")</f>
         <v>21</v>
       </c>
-      <c r="E47" s="0" t="n">
-        <f aca="false">COUNTIF((B2:AY2~ B13:AY13~ B24:AY24), "")</f>
-        <v>25</v>
+      <c r="D47" s="44" t="s">
+        <v>234</v>
+      </c>
+      <c r="E47" s="48" t="n">
+        <f aca="false">COUNTIF((B11:AY11~ B22:AY22~ B33:AY33~ B44:AY44), "No")</f>
+        <v>53</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="J47" s="0" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="47" t="s">
+      <c r="A48" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="B48" s="48" t="n">
+      <c r="B48" s="47" t="n">
         <f aca="false">COUNTIF((B3:AY4~B14:AY15~B25:AY26~B36:AY37),"Water")</f>
         <v>21</v>
       </c>
-      <c r="E48" s="0" t="n">
-        <f aca="false">COUNTIF(B35:AY35,"")</f>
-        <v>13</v>
-      </c>
       <c r="J48" s="0" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="47" t="s">
+      <c r="A49" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B49" s="48" t="n">
+      <c r="B49" s="47" t="n">
         <f aca="false">COUNTIF((B3:AY4~B14:AY15~B25:AY26~B36:AY37),"Fire")</f>
         <v>15</v>
       </c>
@@ -6739,10 +6631,10 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="47" t="s">
+      <c r="A50" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="B50" s="48" t="n">
+      <c r="B50" s="47" t="n">
         <f aca="false">COUNTIF((B3:AY4~B14:AY15~B25:AY26~B36:AY37),"Grass")</f>
         <v>19</v>
       </c>
@@ -6751,10 +6643,10 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="47" t="s">
+      <c r="A51" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="B51" s="48" t="n">
+      <c r="B51" s="47" t="n">
         <f aca="false">COUNTIF((B3:AY4~B14:AY15~B25:AY26~B36:AY37),"Electric")</f>
         <v>11</v>
       </c>
@@ -6763,10 +6655,10 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="47" t="s">
+      <c r="A52" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="B52" s="48" t="n">
+      <c r="B52" s="47" t="n">
         <f aca="false">COUNTIF((B3:AY4~B14:AY15~B25:AY26~B36:AY37),"Fighting")</f>
         <v>12</v>
       </c>
@@ -6775,10 +6667,10 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="47" t="s">
+      <c r="A53" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="B53" s="48" t="n">
+      <c r="B53" s="47" t="n">
         <f aca="false">COUNTIF((B3:AY4~B14:AY15~B25:AY26~B36:AY37),"Psychic")</f>
         <v>16</v>
       </c>
@@ -6787,10 +6679,10 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="47" t="s">
+      <c r="A54" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="B54" s="48" t="n">
+      <c r="B54" s="47" t="n">
         <f aca="false">COUNTIF((B3:AY4~B14:AY15~B25:AY26~B36:AY37),"Ghost")</f>
         <v>11</v>
       </c>
@@ -6799,10 +6691,10 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="47" t="s">
+      <c r="A55" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="B55" s="48" t="n">
+      <c r="B55" s="47" t="n">
         <f aca="false">COUNTIF((B3:AY4~B14:AY15~B25:AY26~B36:AY37),"Ice")</f>
         <v>14</v>
       </c>
@@ -6811,10 +6703,10 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="47" t="s">
+      <c r="A56" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="B56" s="48" t="n">
+      <c r="B56" s="47" t="n">
         <f aca="false">COUNTIF((B3:AY4~B14:AY15~B25:AY26~B36:AY37),"Flying")</f>
         <v>26</v>
       </c>
@@ -6823,10 +6715,10 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="47" t="s">
+      <c r="A57" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="B57" s="48" t="n">
+      <c r="B57" s="47" t="n">
         <f aca="false">COUNTIF((B3:AY4~B14:AY15~B25:AY26~B36:AY37),"Poison")</f>
         <v>17</v>
       </c>
@@ -6835,10 +6727,10 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="47" t="s">
+      <c r="A58" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="B58" s="48" t="n">
+      <c r="B58" s="47" t="n">
         <f aca="false">COUNTIF((B3:AY4~B14:AY15~B25:AY26~B36:AY37),"Ground")</f>
         <v>22</v>
       </c>
@@ -6847,10 +6739,10 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="47" t="s">
+      <c r="A59" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="B59" s="48" t="n">
+      <c r="B59" s="47" t="n">
         <f aca="false">COUNTIF((B3:AY4~B14:AY15~B25:AY26~B36:AY37),"Bug")</f>
         <v>18</v>
       </c>
@@ -6859,10 +6751,10 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="47" t="s">
+      <c r="A60" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="B60" s="48" t="n">
+      <c r="B60" s="47" t="n">
         <f aca="false">COUNTIF((B3:AY4~B14:AY15~B25:AY26~B36:AY37),"Rock")</f>
         <v>10</v>
       </c>
@@ -6871,10 +6763,10 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="47" t="s">
+      <c r="A61" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="B61" s="48" t="n">
+      <c r="B61" s="47" t="n">
         <f aca="false">COUNTIF((B3:AY4~B14:AY15~B25:AY26~B36:AY37),"Dragon")</f>
         <v>10</v>
       </c>
@@ -6883,7 +6775,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="47" t="s">
+      <c r="A62" s="46" t="s">
         <v>44</v>
       </c>
       <c r="B62" s="49" t="n">
@@ -6895,10 +6787,10 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="47" t="s">
+      <c r="A63" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="B63" s="48" t="n">
+      <c r="B63" s="47" t="n">
         <f aca="false">COUNTIF((B3:AY4~B14:AY15~B25:AY26~B36:AY37),"Steel")</f>
         <v>11</v>
       </c>
@@ -6960,121 +6852,121 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J73" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J74" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J75" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J76" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="52"/>
       <c r="D77" s="52"/>
       <c r="J77" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="52"/>
       <c r="D78" s="52"/>
       <c r="J78" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="52"/>
       <c r="D79" s="52"/>
       <c r="J79" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J80" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="52"/>
       <c r="D81" s="52"/>
       <c r="J81" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="52"/>
       <c r="D82" s="52"/>
       <c r="J82" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="52"/>
       <c r="D83" s="52"/>
       <c r="J83" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="52"/>
       <c r="D84" s="52"/>
       <c r="J84" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="52"/>
       <c r="D85" s="52"/>
       <c r="J85" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="52"/>
       <c r="D86" s="52"/>
       <c r="J86" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="52"/>
       <c r="D87" s="52"/>
       <c r="J87" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="52"/>
       <c r="D88" s="52"/>
       <c r="J88" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J89" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="52"/>
       <c r="D90" s="52"/>
       <c r="J90" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J91" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>